<commit_message>
20200502 - atualização de planilha
atualização da planilha
</commit_message>
<xml_diff>
--- a/Planilhas/Testes de Avaliação do Classificador.xlsx
+++ b/Planilhas/Testes de Avaliação do Classificador.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LabDataScience\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77718C7A-740B-41D1-A136-94FBFB0B7D83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADF7B0D-F529-45FB-ABCC-93E4544FB87D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{21FBC840-F5F1-4CAB-B87B-4589D1B93DC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Teste 01 Iris Flower com KNN" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t xml:space="preserve">SETOSA </t>
   </si>
@@ -175,12 +175,15 @@
   <si>
     <t>ESPECIFICIDADE</t>
   </si>
+  <si>
+    <t>Teste 01 - Iris Flower com KNN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +224,14 @@
     <font>
       <i/>
       <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -300,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -308,7 +319,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -339,33 +349,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -374,6 +381,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -690,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD3ED41-B67C-4C45-857D-4B54CADC8A9B}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:J19"/>
+      <selection activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,307 +725,317 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F3" s="27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B4" s="7">
         <v>16</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C4" s="7">
         <v>44</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D4" s="7">
         <v>0</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E4" s="10">
         <v>0</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F4" s="10">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B5" s="8">
         <v>22</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C5" s="8">
         <v>34</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D5" s="8">
         <v>3</v>
       </c>
-      <c r="E3" s="9">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9">
         <v>18</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C6" s="9">
         <v>38</v>
       </c>
-      <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
         <v>3</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F6" s="9">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13">
-        <f>SUM(F2:F4)</f>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12">
+        <f>SUM(F4:F6)</f>
         <v>60</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G8" s="25" t="s">
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H10" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="I10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J10" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G9" s="27" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="22">
-        <f>B2/(B2+D2)</f>
-        <v>1</v>
-      </c>
-      <c r="I9" s="22">
-        <f>C2/(C2+E2)</f>
-        <v>1</v>
-      </c>
-      <c r="J9" s="14">
-        <f>2*H9*I9/(H9+I9)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="4"/>
-      <c r="G10" s="27" t="s">
+      <c r="H11" s="20">
+        <f>B4/(B4+D4)</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="20">
+        <f>C4/(C4+E4)</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="13">
+        <f>2*H11*I11/(H11+I11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="4"/>
+      <c r="G12" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="22">
-        <f>B3/(B3+D3)</f>
+      <c r="H12" s="20">
+        <f>B5/(B5+D5)</f>
         <v>0.88</v>
       </c>
-      <c r="I10" s="22">
-        <f>B3/(B3+E3)</f>
+      <c r="I12" s="20">
+        <f>B5/(B5+E5)</f>
         <v>0.95652173913043481</v>
       </c>
-      <c r="J10" s="14">
-        <f t="shared" ref="J10:J11" si="0">2*H10*I10/(H10+I10)</f>
+      <c r="J12" s="13">
+        <f t="shared" ref="J12:J13" si="0">2*H12*I12/(H12+I12)</f>
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="23">
-        <f>B4/(B4+D4)</f>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="21">
+        <f>B6/(B6+D6)</f>
         <v>0.94736842105263153</v>
       </c>
-      <c r="I11" s="23">
-        <f>B4/(B4+E4)</f>
+      <c r="I13" s="21">
+        <f>B6/(B6+E6)</f>
         <v>0.8571428571428571</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J13" s="13">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="G12" s="25" t="s">
+    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="G14" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H14" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J14" s="22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G13" s="27" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G15" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="15">
-        <f>(D2+E2)/(B2+C2+D2+E2)</f>
+      <c r="H15" s="14">
+        <f>(D4+E4)/(B4+C4+D4+E4)</f>
         <v>0</v>
-      </c>
-      <c r="I13" s="20">
-        <f>1-H13</f>
-        <v>1</v>
-      </c>
-      <c r="J13" s="20">
-        <f>C2/(C2+D2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="17">
-        <f>(D3+E3)/(B3+C3+D3+E3)</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="I14" s="18">
-        <f>1-H14</f>
-        <v>0.93333333333333335</v>
-      </c>
-      <c r="J14" s="18">
-        <f t="shared" ref="J14:J15" si="1">C3/(C3+D3)</f>
-        <v>0.91891891891891897</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G15" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="17">
-        <f>(D4+E4)/(B4+C4+D4+E4)</f>
-        <v>6.6666666666666666E-2</v>
       </c>
       <c r="I15" s="18">
         <f>1-H15</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="18">
+        <f>C4/(C4+D4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G16" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="15">
+        <f>(D5+E5)/(B5+C5+D5+E5)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I16" s="16">
+        <f>1-H16</f>
         <v>0.93333333333333335</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J16" s="16">
+        <f t="shared" ref="J16:J17" si="1">C5/(C5+D5)</f>
+        <v>0.91891891891891897</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="15">
+        <f>(D6+E6)/(B6+C6+D6+E6)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I17" s="16">
+        <f>1-H17</f>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="J17" s="16">
         <f t="shared" si="1"/>
         <v>0.97435897435897434</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G16" s="25" t="s">
+    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G18" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H18" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="I18" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="16" t="s">
+      <c r="J18" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G17" s="27" t="s">
+    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G19" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="15">
-        <f>1-J13</f>
+      <c r="H19" s="14">
+        <f>1-J15</f>
         <v>0</v>
       </c>
-      <c r="I17" s="20">
-        <f>B2/(B2+D2)</f>
-        <v>1</v>
-      </c>
-      <c r="J17" s="20">
-        <f>C2/(C2+E2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G18" s="27" t="s">
+      <c r="I19" s="18">
+        <f>B4/(B4+D4)</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="18">
+        <f>C4/(C4+E4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G20" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="17">
-        <f t="shared" ref="H18:H19" si="2">1-J14</f>
+      <c r="H20" s="15">
+        <f t="shared" ref="H20:H21" si="2">1-J16</f>
         <v>8.108108108108103E-2</v>
       </c>
-      <c r="I18" s="20">
-        <f>B3/(B3+D3)</f>
+      <c r="I20" s="18">
+        <f>B5/(B5+D5)</f>
         <v>0.88</v>
       </c>
-      <c r="J18" s="18">
-        <f t="shared" ref="J18:J19" si="3">C3/(C3+E3)</f>
+      <c r="J20" s="16">
+        <f t="shared" ref="J20:J21" si="3">C5/(C5+E5)</f>
         <v>0.97142857142857142</v>
       </c>
     </row>
-    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G19" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" s="19">
+    <row r="21" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="17">
         <f t="shared" si="2"/>
         <v>2.5641025641025661E-2</v>
       </c>
-      <c r="I19" s="19">
-        <f>B4/(B4+D4)</f>
+      <c r="I21" s="17">
+        <f>B6/(B6+D6)</f>
         <v>0.94736842105263153</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J21" s="17">
         <f t="shared" si="3"/>
         <v>0.92682926829268297</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>